<commit_message>
PMD GUI parameters from user.
</commit_message>
<xml_diff>
--- a/DGD.xlsx
+++ b/DGD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kavinda Ravishan\source\repos\kavinda-ravishan\GPIB-Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E750F1-4BD4-43CD-94DF-34AC4C17DDD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF874C8A-903B-427C-A5A5-603F7E072C3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="20490" windowHeight="9900" xr2:uid="{6855B79E-CDE9-4816-81B4-887632F1B8D5}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="20490" windowHeight="9900" xr2:uid="{67141159-CB7C-4AC6-A5CD-FAE5CB40CE63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,8 +409,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2910E0-7A39-4181-8F30-70A920D2251A}">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C245B9-0FDE-4347-B195-D3836F2891C3}">
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,7 +430,7 @@
         <v>2</v>
       </c>
       <c r="E1">
-        <v>1560</v>
+        <v>1570</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -588,6 +588,116 @@
       </c>
       <c r="C16" s="1">
         <v>2.0744786499887601E-8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1561</v>
+      </c>
+      <c r="B17" s="1">
+        <v>8.5642638734649905E-8</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2.07713909152692E-8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1562</v>
+      </c>
+      <c r="B18" s="1">
+        <v>8.5752401842750003E-8</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.07980123792982E-8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1563</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8.5862235244228898E-8</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2.0824650891975699E-8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1564</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8.5972138939084301E-8</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2.0851306453301299E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1565</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8.6082112927310401E-8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2.0877979063273401E-8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1566</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8.6192157208910905E-8</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2.0904668721893101E-8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1567</v>
+      </c>
+      <c r="B23" s="1">
+        <v>8.6302271783892601E-8</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2.09313754291619E-8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1568</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8.6412456652258905E-8</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2.0958099185080699E-8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1569</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8.6522711814003E-8</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2.09848399896477E-8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1570</v>
+      </c>
+      <c r="B26" s="1">
+        <v>8.6633037269121407E-8</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2.10115978428623E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mean, Min and Max PMD.
</commit_message>
<xml_diff>
--- a/DGD.xlsx
+++ b/DGD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kavinda Ravishan\source\repos\kavinda-ravishan\GPIB-Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF874C8A-903B-427C-A5A5-603F7E072C3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1A1223-9950-4BDB-8476-E40A13AA8925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="20490" windowHeight="9900" xr2:uid="{67141159-CB7C-4AC6-A5CD-FAE5CB40CE63}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="20490" windowHeight="9900" xr2:uid="{FD6616B5-644D-4598-8BB0-A8E5D0D2ABD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>From</t>
   </si>
@@ -51,13 +51,16 @@
     <t>Km</t>
   </si>
   <si>
-    <t>Wave Lenght (nm)</t>
-  </si>
-  <si>
-    <t>DGD (ps)</t>
-  </si>
-  <si>
-    <t>PMD</t>
+    <t>Mean PMD</t>
+  </si>
+  <si>
+    <t>Minimum PMD</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>Maximum PMD</t>
   </si>
 </sst>
 </file>
@@ -409,8 +412,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C245B9-0FDE-4347-B195-D3836F2891C3}">
-  <dimension ref="A1:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC1B96BB-ED30-487E-99CB-6C38822BFAD2}">
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,7 +433,7 @@
         <v>2</v>
       </c>
       <c r="E1">
-        <v>1570</v>
+        <v>1560</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -458,246 +461,200 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.44335644998176899</v>
+      </c>
+    </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
         <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.0532564928174402E-8</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
+      <c r="D5">
+        <v>1552</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1550</v>
+      <c r="A6" t="s">
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>10.0475453379038</v>
-      </c>
-      <c r="C6">
-        <v>2.43688768860939</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+        <v>2.4400330754427002</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
         <v>1551</v>
       </c>
-      <c r="B7">
-        <v>10.060514100051</v>
-      </c>
-      <c r="C7">
-        <v>2.4400330754427002</v>
+      <c r="E6" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1552</v>
-      </c>
-      <c r="B8" s="1">
-        <v>8.4657933963715903E-8</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2.0532564928174402E-8</v>
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1550</v>
+      </c>
+      <c r="C8">
+        <v>10.0475453379038</v>
+      </c>
+      <c r="D8">
+        <v>2.43688768860939</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1553</v>
-      </c>
-      <c r="B9" s="1">
-        <v>8.4767064431423898E-8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.05590329543705E-8</v>
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>1551</v>
+      </c>
+      <c r="C9">
+        <v>10.060514100051</v>
+      </c>
+      <c r="D9">
+        <v>2.4400330754427002</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1554</v>
-      </c>
-      <c r="B10" s="1">
-        <v>8.4876265192507302E-8</v>
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1552</v>
       </c>
       <c r="C10" s="1">
-        <v>2.05855180292143E-8</v>
+        <v>8.4657933963715903E-8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2.0532564928174402E-8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1555</v>
-      </c>
-      <c r="B11" s="1">
-        <v>8.49855362469629E-8</v>
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>1553</v>
       </c>
       <c r="C11" s="1">
-        <v>2.0612020152705101E-8</v>
+        <v>8.4767064431423898E-8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2.05590329543705E-8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1556</v>
-      </c>
-      <c r="B12" s="1">
-        <v>8.5094877594804494E-8</v>
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1554</v>
       </c>
       <c r="C12" s="1">
-        <v>2.06385393248462E-8</v>
+        <v>8.4876265192507302E-8</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2.05855180292143E-8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1557</v>
-      </c>
-      <c r="B13" s="1">
-        <v>8.5204289236027004E-8</v>
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>1555</v>
       </c>
       <c r="C13" s="1">
-        <v>2.0665075545636302E-8</v>
+        <v>8.49855362469629E-8</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2.0612020152705101E-8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1558</v>
-      </c>
-      <c r="B14" s="1">
-        <v>8.5313771170609305E-8</v>
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>1556</v>
       </c>
       <c r="C14" s="1">
-        <v>2.0691628815070399E-8</v>
+        <v>8.5094877594804494E-8</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.06385393248462E-8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1559</v>
-      </c>
-      <c r="B15" s="1">
-        <v>8.54233233985764E-8</v>
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>1557</v>
       </c>
       <c r="C15" s="1">
-        <v>2.07181991331545E-8</v>
+        <v>8.5204289236027004E-8</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.0665075545636302E-8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>1558</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8.5313771170609305E-8</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2.0691628815070399E-8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>1559</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8.54233233985764E-8</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.07181991331545E-8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
         <v>1560</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C18" s="1">
         <v>8.5532945919923694E-8</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D18" s="1">
         <v>2.0744786499887601E-8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1561</v>
-      </c>
-      <c r="B17" s="1">
-        <v>8.5642638734649905E-8</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2.07713909152692E-8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1562</v>
-      </c>
-      <c r="B18" s="1">
-        <v>8.5752401842750003E-8</v>
-      </c>
-      <c r="C18" s="1">
-        <v>2.07980123792982E-8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1563</v>
-      </c>
-      <c r="B19" s="1">
-        <v>8.5862235244228898E-8</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2.0824650891975699E-8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1564</v>
-      </c>
-      <c r="B20" s="1">
-        <v>8.5972138939084301E-8</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2.0851306453301299E-8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1565</v>
-      </c>
-      <c r="B21" s="1">
-        <v>8.6082112927310401E-8</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2.0877979063273401E-8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1566</v>
-      </c>
-      <c r="B22" s="1">
-        <v>8.6192157208910905E-8</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2.0904668721893101E-8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1567</v>
-      </c>
-      <c r="B23" s="1">
-        <v>8.6302271783892601E-8</v>
-      </c>
-      <c r="C23" s="1">
-        <v>2.09313754291619E-8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1568</v>
-      </c>
-      <c r="B24" s="1">
-        <v>8.6412456652258905E-8</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2.0958099185080699E-8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1569</v>
-      </c>
-      <c r="B25" s="1">
-        <v>8.6522711814003E-8</v>
-      </c>
-      <c r="C25" s="1">
-        <v>2.09848399896477E-8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1570</v>
-      </c>
-      <c r="B26" s="1">
-        <v>8.6633037269121407E-8</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2.10115978428623E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Load excel and show data.
</commit_message>
<xml_diff>
--- a/DGD.xlsx
+++ b/DGD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kavinda Ravishan\source\repos\kavinda-ravishan\GPIB-Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C5524D-AA96-43E6-8D7A-42E2D7D3C468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAC3C3C-0813-45C5-9B28-1D24902DE8BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="20490" windowHeight="9900" xr2:uid="{A6423802-0665-42FC-B8BB-E6E5C79507BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{A6423802-0665-42FC-B8BB-E6E5C79507BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>From</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Maximum PMD</t>
+  </si>
+  <si>
+    <t>Wave Lenght (nm)</t>
+  </si>
+  <si>
+    <t>DGD (ps)</t>
+  </si>
+  <si>
+    <t>PMD</t>
   </si>
 </sst>
 </file>
@@ -96,9 +105,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,11 +423,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C49E149-9971-45FF-AC3A-DC010AC9BE78}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -466,21 +483,24 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.44335644998176899</v>
+        <f>AVERAGE(D9:D19)</f>
+        <v>0.55946795061790178</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
-        <v>2.0532564928174402E-8</v>
+      <c r="B5" s="2">
+        <f>D19</f>
+        <v>0.46734189588251002</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5">
-        <v>1552</v>
+        <f>B19</f>
+        <v>1560</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -491,173 +511,209 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>2.4400330754427002</v>
+        <f>D17</f>
+        <v>0.7006611671674623</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6">
-        <v>1551</v>
+        <f>B17</f>
+        <v>1558</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>1550</v>
-      </c>
-      <c r="C8">
-        <v>10.0475453379038</v>
-      </c>
-      <c r="D8">
-        <v>2.43688768860939</v>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>1551</v>
-      </c>
-      <c r="C9">
-        <v>10.060514100051</v>
+        <v>1550</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.2315999999999998</v>
       </c>
       <c r="D9">
-        <v>2.4400330754427002</v>
-      </c>
+        <f>C9/SQRT(B3)</f>
+        <v>0.54124250083108061</v>
+      </c>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>1552</v>
-      </c>
-      <c r="C10" s="1">
-        <v>8.4657933963715903E-8</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2.0532564928174402E-8</v>
-      </c>
+        <v>1551</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.2778</v>
+      </c>
+      <c r="D10">
+        <f>C10/SQRT(B3)</f>
+        <v>0.55244764670775925</v>
+      </c>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>1553</v>
-      </c>
-      <c r="C11" s="1">
-        <v>8.4767064431423898E-8</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2.05590329543705E-8</v>
-      </c>
+        <v>1552</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.2865000000000002</v>
+      </c>
+      <c r="D11">
+        <f>C11/SQRT(B3)</f>
+        <v>0.55455770664557535</v>
+      </c>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>1554</v>
-      </c>
-      <c r="C12" s="1">
-        <v>8.4876265192507302E-8</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2.05855180292143E-8</v>
-      </c>
+        <v>1553</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2.2168999999999999</v>
+      </c>
+      <c r="D12">
+        <f>C12/SQRT(B3)</f>
+        <v>0.53767722714304655</v>
+      </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>1555</v>
-      </c>
-      <c r="C13" s="1">
-        <v>8.49855362469629E-8</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2.0612020152705101E-8</v>
-      </c>
+        <v>1554</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2.2389000000000001</v>
+      </c>
+      <c r="D13">
+        <f>C13/SQRT(B3)</f>
+        <v>0.5430130108938459</v>
+      </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>1556</v>
-      </c>
-      <c r="C14" s="1">
-        <v>8.5094877594804494E-8</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2.06385393248462E-8</v>
-      </c>
+        <v>1555</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2.2442000000000002</v>
+      </c>
+      <c r="D14">
+        <f>C14/SQRT(B3)</f>
+        <v>0.54429844970653851</v>
+      </c>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>1557</v>
-      </c>
-      <c r="C15" s="1">
-        <v>8.5204289236027004E-8</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2.0665075545636302E-8</v>
-      </c>
+        <v>1556</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2.1282000000000001</v>
+      </c>
+      <c r="D15">
+        <f>C15/SQRT(B3)</f>
+        <v>0.51616431720232381</v>
+      </c>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>1557</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2.1219000000000001</v>
+      </c>
+      <c r="D16">
+        <f>C16/SQRT(B3)</f>
+        <v>0.51463634276459491</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>9</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>1558</v>
       </c>
-      <c r="C16" s="1">
-        <v>8.5313771170609305E-8</v>
-      </c>
-      <c r="D16" s="1">
-        <v>2.0691628815070399E-8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="C17" s="2">
+        <v>2.8889</v>
+      </c>
+      <c r="D17">
+        <f>C17/SQRT(B3)</f>
+        <v>0.7006611671674623</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>10</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>1559</v>
       </c>
-      <c r="C17" s="1">
-        <v>8.54233233985764E-8</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2.07181991331545E-8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="C18" s="2">
+        <v>2.8123999999999998</v>
+      </c>
+      <c r="D18">
+        <f>C18/SQRT(B3)</f>
+        <v>0.68210719185218283</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>11</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>1560</v>
       </c>
-      <c r="C18" s="1">
-        <v>8.5532945919923694E-8</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2.0744786499887601E-8</v>
-      </c>
+      <c r="C19" s="2">
+        <v>1.9269000000000001</v>
+      </c>
+      <c r="D19">
+        <f>C19/SQRT(B3)</f>
+        <v>0.46734189588251002</v>
+      </c>
+      <c r="E19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>